<commit_message>
22-11 CCodes com reset
</commit_message>
<xml_diff>
--- a/Spec/ControlUnitSignals.xlsx
+++ b/Spec/ControlUnitSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="67">
   <si>
     <t xml:space="preserve">Datapath</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">i_DLen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i_Ccload</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
@@ -394,25 +397,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:S19"/>
+  <dimension ref="C4:T20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,19 +456,22 @@
       <c r="S4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="T4" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="8" t="n">
         <v>0</v>
@@ -474,31 +480,34 @@
         <v>0</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,13 +515,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="8" t="n">
         <v>0</v>
@@ -521,31 +530,34 @@
         <v>0</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,13 +565,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I7" s="8" t="n">
         <v>0</v>
@@ -568,31 +580,34 @@
         <v>0</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T7" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,13 +615,13 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I8" s="8" t="n">
         <v>0</v>
@@ -615,45 +630,48 @@
         <v>0</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T8" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I9" s="8" t="n">
         <v>0</v>
@@ -662,31 +680,34 @@
         <v>0</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T9" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,10 +716,10 @@
       </c>
       <c r="D10" s="3"/>
       <c r="G10" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="8" t="n">
         <v>0</v>
@@ -707,31 +728,34 @@
         <v>0</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T10" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,10 +764,10 @@
       </c>
       <c r="D11" s="3"/>
       <c r="G11" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I11" s="8" t="n">
         <v>0</v>
@@ -752,31 +776,34 @@
         <v>0</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T11" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,10 +812,10 @@
       </c>
       <c r="D12" s="3"/>
       <c r="G12" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I12" s="8" t="n">
         <v>1</v>
@@ -797,31 +824,34 @@
         <v>0</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,43 +860,46 @@
       </c>
       <c r="D13" s="3"/>
       <c r="G13" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J13" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T13" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,43 +908,46 @@
       </c>
       <c r="D14" s="3"/>
       <c r="G14" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="P14" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T14" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,10 +956,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="G15" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" s="8" t="n">
         <v>0</v>
@@ -932,31 +968,34 @@
         <v>0</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T15" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,51 +1004,54 @@
       </c>
       <c r="D16" s="3"/>
       <c r="G16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="Q16" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I17" s="8" t="n">
         <v>0</v>
@@ -1018,39 +1060,42 @@
         <v>0</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T17" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G18" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I18" s="8" t="n">
         <v>0</v>
@@ -1059,39 +1104,42 @@
         <v>0</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I19" s="8" t="n">
         <v>0</v>
@@ -1100,33 +1148,37 @@
         <v>0</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
+        <v>24</v>
+      </c>
+      <c r="T19" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:D4"/>

</xml_diff>